<commit_message>
chemcurier v.0.9.3 table in excel creation v.1.5 with download at 31/10/2023
</commit_message>
<xml_diff>
--- a/src/ChemcourierProgr.xlsx
+++ b/src/ChemcourierProgr.xlsx
@@ -34,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +42,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,621 +436,631 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Бренд</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Получатель</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, шт.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, USD</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Средневзвешенная цена реализации единицы товара, USD</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, шт.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, USD</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>Средневзвешенная цена реализации единицы товара, USD</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, шт.</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, USD</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>Средневзвешенная цена реализации единицы товара, USD</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, шт.</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>Объем поставки, USD</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>Средневзвешенная цена реализации единицы товара, USD</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>количество, шт.</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>сумма импорта долл.США без НДС</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>средневзвешенная цена, долл. США без НДС</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>Continental</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Римэкс-Шины</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>1 880</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>56 395.02</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>30.0</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>600</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>19 416.52</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>32.36</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
         <is>
           <t>600</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" s="1" t="inlineStr">
         <is>
           <t>19 416.52</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>32.36</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P3" s="1" t="inlineStr">
         <is>
           <t>3 080</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" s="1" t="inlineStr">
         <is>
           <t>95 228.06</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R3" s="1" t="inlineStr">
         <is>
           <t>30.92</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>Nexen</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>ПКФ ПИН</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>4 060</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>113 129.39</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>27.86</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>1 720</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>49 887.12</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>29.0</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>49 887.12</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" s="1" t="inlineStr">
         <is>
           <t>498.87</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="P4" s="1" t="inlineStr">
         <is>
           <t>5 880</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>212 903.63</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" s="1" t="inlineStr">
         <is>
           <t>36.21</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>Nexen</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Северный Путь</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>2 160</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>58 893.54</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>27.27</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="1" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>15 826.65</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>31.65</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M5" s="1" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" s="1" t="inlineStr">
         <is>
           <t>15 826.65</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O5" s="1" t="inlineStr">
         <is>
           <t>31.65</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P5" s="1" t="inlineStr">
         <is>
           <t>3 160</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" s="1" t="inlineStr">
         <is>
           <t>90 546.84</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R5" s="1" t="inlineStr">
         <is>
           <t>28.65</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>Nexen</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>Союзоптторг</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
         <is>
           <t>320</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>9 520.52</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="1" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M6" s="1" t="inlineStr">
         <is>
           <t>320</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="N6" s="1" t="inlineStr">
         <is>
           <t>9 520.52</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="O6" s="1" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="P6" s="1" t="inlineStr">
         <is>
           <t>640</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q6" s="1" t="inlineStr">
         <is>
           <t>19 041.04</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="R6" s="1" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>Roadstone</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>Сталкер</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>1 900</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>52 664.13</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>27.72</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="1" t="inlineStr">
         <is>
           <t>4 932</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="1" t="inlineStr">
         <is>
           <t>136 202.83</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="1" t="inlineStr">
         <is>
           <t>27.62</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" s="1" t="inlineStr">
         <is>
           <t>1 096</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" s="1" t="inlineStr">
         <is>
           <t>22 868.96</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" s="1" t="inlineStr">
         <is>
           <t>20.87</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M7" s="1" t="inlineStr">
         <is>
           <t>4 932</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="N7" s="1" t="inlineStr">
         <is>
           <t>136 202.83</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="O7" s="1" t="n"/>
+      <c r="P7" s="1" t="inlineStr">
         <is>
           <t>12 860</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="Q7" s="1" t="inlineStr">
         <is>
           <t>347 938.75</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="R7" s="1" t="inlineStr">
         <is>
           <t>27.06</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>ИТОГО</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>10 000</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="1" t="inlineStr">
         <is>
           <t>281 082.08</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="1" t="inlineStr">
         <is>
           <t>28.11</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="1" t="inlineStr">
         <is>
           <t>8 072</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="1" t="inlineStr">
         <is>
           <t>230 853.64</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="1" t="inlineStr">
         <is>
           <t>28.6</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" s="1" t="inlineStr">
         <is>
           <t>1 096</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="K8" s="1" t="inlineStr">
         <is>
           <t>22 868.96</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" s="1" t="inlineStr">
         <is>
           <t>20.87</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M8" s="1" t="inlineStr">
         <is>
           <t>6 452</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="N8" s="1" t="inlineStr">
         <is>
           <t>230 853.64</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="O8" s="1" t="inlineStr">
         <is>
           <t>35.78</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="P8" s="1" t="inlineStr">
         <is>
           <t>25 620</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="Q8" s="1" t="inlineStr">
         <is>
           <t>765 658.32</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="R8" s="1" t="inlineStr">
         <is>
           <t>29.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Согласно данным информационно-аналитическго агентства «Хим-Курьер»</t>
         </is>
       </c>
     </row>

</xml_diff>